<commit_message>
TP-7 [RPA Developer] Parse google form results
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIpath_projects\TripPlanner\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F33525-927A-4046-8D5A-CC22DB1986D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A6E505-AFFC-40FF-B7B1-18FE9405CD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -88,20 +88,12 @@
   </si>
   <si>
     <t>Framework</t>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
   </si>
   <si>
@@ -120,12 +112,6 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
     <t>MaxConsecutiveSystemExceptions</t>
   </si>
   <si>
@@ -159,9 +145,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
     <t>EmailCredentials</t>
   </si>
   <si>
@@ -184,6 +167,45 @@
   </si>
   <si>
     <t xml:space="preserve">Trip-Planner Robot Registration Response Letter Subject </t>
+  </si>
+  <si>
+    <t>UserTripPrefResponsesURL</t>
+  </si>
+  <si>
+    <t>UserResponsesURL</t>
+  </si>
+  <si>
+    <t>This is URL for site with responses of users</t>
+  </si>
+  <si>
+    <t>OrchestratorEmailQueueName</t>
+  </si>
+  <si>
+    <t>Registration_Emails</t>
+  </si>
+  <si>
+    <t>Each transaction in this queue is a transaction with the email address of the user waiting for the registration response email.</t>
+  </si>
+  <si>
+    <t>OrchestratorEmailQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name.</t>
+  </si>
+  <si>
+    <t>Trip-Planner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each item in this queue is request from user to find best matching trip </t>
+  </si>
+  <si>
+    <t>Trip_Planning_Requests</t>
+  </si>
+  <si>
+    <t>OrchestratorPlanningRequestsQueueName</t>
+  </si>
+  <si>
+    <t>OrchestratorPlanningRequestsQueueFolder</t>
   </si>
 </sst>
 </file>
@@ -569,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -617,82 +639,114 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="14.4">
       <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.4">
+      <c r="A5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>52</v>
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
         <v>49</v>
       </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1745,18 +1799,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1780,7 +1834,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1802,7 +1856,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1813,7 +1867,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1824,53 +1878,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2854,7 +2908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2874,7 +2928,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>